<commit_message>
Update on 3 phase rectifier selection
</commit_message>
<xml_diff>
--- a/Component Selection/BOM.xlsx
+++ b/Component Selection/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Civan Serhat Çevik\Desktop\24Fall\463\Term Project\463-Term-Project\Component Selection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\batuh\Desktop\Lectrues 4-1\EE463\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDD5F29-93E0-4F18-93B2-0BC1D16AC3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9516"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Komponent</t>
   </si>
@@ -67,13 +67,28 @@
   </si>
   <si>
     <t>Switch</t>
+  </si>
+  <si>
+    <t>SKBPC5004 Three Phase Bridge Rectifier</t>
+  </si>
+  <si>
+    <t>Yok</t>
+  </si>
+  <si>
+    <t>https://www.motorobit.com/skbpc5016-50a-1600v-trifaze-kopru-diyot-3-faz</t>
+  </si>
+  <si>
+    <t>1600V</t>
+  </si>
+  <si>
+    <t>50A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +108,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +127,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -117,14 +146,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -141,17 +174,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1EF04FB-E8F6-4E24-83BB-6CE57F34A57F}" name="Table1" displayName="Table1" ref="A2:H29" totalsRowShown="0">
-  <autoFilter ref="A2:H29" xr:uid="{F1EF04FB-E8F6-4E24-83BB-6CE57F34A57F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H29" totalsRowShown="0">
+  <autoFilter ref="A2:H29"/>
   <tableColumns count="8">
-    <tableColumn id="15" xr3:uid="{EE133555-D594-4C7C-8D1D-A03AA961AD66}" name="Tipi"/>
-    <tableColumn id="1" xr3:uid="{57E01DC7-E995-4C7B-9FC9-1A0B2BD73817}" name="Komponent"/>
-    <tableColumn id="2" xr3:uid="{7137AB8A-8455-4599-98E2-C10308118B8D}" name="Adet"/>
-    <tableColumn id="3" xr3:uid="{379524DE-0D65-4C7E-9612-F3FE5F50ABFF}" name="Labda var mı?"/>
-    <tableColumn id="4" xr3:uid="{02F3DE5F-220B-4CB0-A2EA-6243577DC7AE}" name="Fiyat"/>
-    <tableColumn id="5" xr3:uid="{EFD07F10-84E0-42CC-88F1-895E6D3D0677}" name="Link"/>
-    <tableColumn id="6" xr3:uid="{E9D857D4-D7B9-414A-A0E3-7D504A88FB7F}" name="Voltage Rating"/>
-    <tableColumn id="7" xr3:uid="{FBF73456-4B69-42D0-A623-849FFA3370C9}" name="Current Rating"/>
+    <tableColumn id="15" name="Tipi"/>
+    <tableColumn id="1" name="Komponent"/>
+    <tableColumn id="2" name="Adet"/>
+    <tableColumn id="3" name="Labda var mı?"/>
+    <tableColumn id="4" name="Fiyat"/>
+    <tableColumn id="5" name="Link"/>
+    <tableColumn id="6" name="Voltage Rating"/>
+    <tableColumn id="7" name="Current Rating"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -419,11 +452,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,7 +506,7 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
@@ -481,13 +514,33 @@
       </c>
       <c r="H3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Complete Simulation Report Uploaded
</commit_message>
<xml_diff>
--- a/Component Selection/BOM.xlsx
+++ b/Component Selection/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\batuh\Desktop\Lectrues 4-1\EE463\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Civan Serhat Çevik\Desktop\24Fall\463\Term Project\463-Term-Project\Component Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C311F62E-2931-4DF4-8435-C2924128CA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9516"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Komponent</t>
   </si>
@@ -82,12 +82,87 @@
   </si>
   <si>
     <t>50A</t>
+  </si>
+  <si>
+    <t>Rectifier</t>
+  </si>
+  <si>
+    <t>36MT120 36A 1200V Trifaze Köprü Diyot 3 Faz - Altın Pin</t>
+  </si>
+  <si>
+    <t>https://www.motorobit.com/36mt120-36a-1200v-trifaze-kopru-diyot-3-faz-altin-pin</t>
+  </si>
+  <si>
+    <t>1200 V</t>
+  </si>
+  <si>
+    <t>36A</t>
+  </si>
+  <si>
+    <t>https://www.hatfon.com/urun/powersem-psd-68-16-rectifier-bridges-kopru-trifaze-68a-1600v</t>
+  </si>
+  <si>
+    <t>POWERSEM PSD 68/16 RECTIFIER BRIDGES KÖP</t>
+  </si>
+  <si>
+    <t>68A</t>
+  </si>
+  <si>
+    <t>https://www.ozdisan.com/guc-yari-iletkenleri/diyot-modul-diyot-dogrultucular/hizli-diyotlar/DSEI30-06A</t>
+  </si>
+  <si>
+    <t>37A</t>
+  </si>
+  <si>
+    <t>600V</t>
+  </si>
+  <si>
+    <t>DSEI30-06A</t>
+  </si>
+  <si>
+    <t>Buck Diode</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyot-modul-diyot-dogrultucular/kopru-diyotlar/GUO40-12NO1</t>
+  </si>
+  <si>
+    <t>GUO40-12NO1</t>
+  </si>
+  <si>
+    <t>1200V</t>
+  </si>
+  <si>
+    <t>40A</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Through Hole Rects: https://ozdisan.com/p/473?ids=10212;780950,9693;355004&amp;groupids=10212,9693&amp;propids=780950,355004&amp;sayfaAdedi=20</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/47uf400v-en</t>
+  </si>
+  <si>
+    <t>400 V</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>47uF 400V</t>
+  </si>
+  <si>
+    <t>IXGH30N60C2</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/igbtler/discrete-igbtler/IXGH30N60C2/336872</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -174,17 +249,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H29" totalsRowShown="0">
-  <autoFilter ref="A2:H29"/>
-  <tableColumns count="8">
-    <tableColumn id="15" name="Tipi"/>
-    <tableColumn id="1" name="Komponent"/>
-    <tableColumn id="2" name="Adet"/>
-    <tableColumn id="3" name="Labda var mı?"/>
-    <tableColumn id="4" name="Fiyat"/>
-    <tableColumn id="5" name="Link"/>
-    <tableColumn id="6" name="Voltage Rating"/>
-    <tableColumn id="7" name="Current Rating"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:I29" totalsRowShown="0">
+  <autoFilter ref="A2:I29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I8">
+    <sortCondition ref="A2:A29"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Tipi"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Komponent"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Adet"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Labda var mı?"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fiyat"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Link"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Voltage Rating"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Current Rating"/>
+    <tableColumn id="8" xr3:uid="{44177463-55F5-4229-B6FA-206F78EDF6C2}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -452,11 +531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +549,7 @@
     <col min="8" max="8" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -495,35 +574,44 @@
       <c r="H2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G4" t="s">
@@ -531,16 +619,147 @@
       </c>
       <c r="H4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{4AD9348B-FB94-4C1E-AAF0-C84DB5D5DCB8}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{F99DDC0A-F1B5-4893-BFA6-F9B35EDE6D25}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{69B7EEB2-61A9-42D3-9AA8-177BD8A1EF68}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{C04626E1-6E8E-4BAE-80C6-35C35CC984E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>